<commit_message>
[UPDATE] repurpose views input
</commit_message>
<xml_diff>
--- a/app/utilities/calificaciones1.xlsx
+++ b/app/utilities/calificaciones1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Desktop\Lyra\app\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCE7A2E-B0A0-4D9C-8E11-DC36A7D9CABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18182571-1564-4AE5-AE12-18D809D9975E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1028,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="63" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
[ADD} lo de andre
</commit_message>
<xml_diff>
--- a/app/utilities/calificaciones1.xlsx
+++ b/app/utilities/calificaciones1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Desktop\Lyra\app\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF558CC-6FE4-46B2-9559-2122052172AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABCE8DC-C66E-46FF-9473-C76B5B6301E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="198">
   <si>
     <t>Matemáticas y emprendimiento</t>
   </si>
@@ -1026,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CD1000"/>
+  <dimension ref="A1:CE1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="BM1" zoomScale="63" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="BX8" sqref="BX8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1040,7 +1040,7 @@
     <col min="11" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1053,242 +1053,245 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AS1" s="13">
-        <v>45592</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="AU1" s="13">
-        <v>45593</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="AW1" s="13">
-        <v>45594</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AY1" s="13">
-        <v>45595</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="BA1" s="13">
-        <v>45596</v>
-      </c>
-      <c r="BB1" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="BC1" s="13">
-        <v>45597</v>
-      </c>
-      <c r="BD1" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="BE1" s="13">
-        <v>45598</v>
-      </c>
-      <c r="BF1" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="BG1" s="13">
-        <v>45599</v>
-      </c>
-      <c r="BH1" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="BI1" s="13">
-        <v>45600</v>
-      </c>
-      <c r="BJ1" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="BK1" s="13">
-        <v>45601</v>
-      </c>
-      <c r="BL1" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="BM1" s="13">
-        <v>45602</v>
-      </c>
-      <c r="BN1" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="BO1" s="13">
-        <v>45603</v>
-      </c>
-      <c r="BP1" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="BQ1" s="13">
-        <v>45604</v>
-      </c>
-      <c r="BR1" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="BS1" s="13">
-        <v>45605</v>
-      </c>
-      <c r="BT1" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="BU1" s="13">
-        <v>45606</v>
-      </c>
-      <c r="BV1" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="BW1" s="13">
-        <v>45607</v>
-      </c>
-      <c r="BX1" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="BY1" s="13">
-        <v>45608</v>
-      </c>
-      <c r="BZ1" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="CA1" s="13">
-        <v>45609</v>
-      </c>
-      <c r="CB1" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="CC1" s="13">
-        <v>45610</v>
-      </c>
-      <c r="CD1" s="2" t="s">
-        <v>197</v>
+      <c r="E1" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="W1" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="X1" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y1" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z1" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB1" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="AC1" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD1" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF1" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="AG1" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="AI1" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ1" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK1" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="AL1" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="AM1" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="AN1" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="AO1" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="AP1" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="AQ1" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR1" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="AS1" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="AT1" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="AU1" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="AV1" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="AW1" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="AX1" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="AY1" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="AZ1" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="BA1" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="BB1" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="BC1" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="BD1" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="BE1" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="BF1" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="BG1" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="BH1" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="BI1" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="BJ1" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="BK1" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="BL1" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="BM1" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="BN1" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="BO1" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="BP1" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="BQ1" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="BR1" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="BS1" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="BT1" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="BU1" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="BV1" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="BW1" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="BX1" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="BY1" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="BZ1" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="CA1" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="CB1" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="CC1" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="CD1" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="CE1" s="12" t="s">
+        <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1301,242 +1304,245 @@
       <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="F2" s="12" t="s">
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AS2" s="13">
+        <v>45592</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="AU2" s="13">
+        <v>45593</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AW2" s="13">
+        <v>45594</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="AY2" s="13">
+        <v>45595</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="BA2" s="13">
+        <v>45596</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="BC2" s="13">
+        <v>45597</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="BE2" s="13">
+        <v>45598</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="BG2" s="13">
+        <v>45599</v>
+      </c>
+      <c r="BH2" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="BI2" s="13">
+        <v>45600</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="BK2" s="13">
+        <v>45601</v>
+      </c>
+      <c r="BL2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="BM2" s="13">
+        <v>45602</v>
+      </c>
+      <c r="BN2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="BO2" s="13">
+        <v>45603</v>
+      </c>
+      <c r="BP2" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="BQ2" s="13">
+        <v>45604</v>
+      </c>
+      <c r="BR2" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="BS2" s="13">
+        <v>45605</v>
+      </c>
+      <c r="BT2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="BU2" s="13">
+        <v>45606</v>
+      </c>
+      <c r="BV2" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="BW2" s="13">
+        <v>45607</v>
+      </c>
+      <c r="BX2" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="BY2" s="13">
+        <v>45608</v>
+      </c>
+      <c r="BZ2" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="CA2" s="13">
+        <v>45609</v>
+      </c>
+      <c r="CB2" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="CC2" s="13">
+        <v>45610</v>
+      </c>
+      <c r="CD2" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="CE2" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q2" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="Z2" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA2" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB2" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="AC2" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="AD2" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="AE2" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="AF2" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="AG2" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="AH2" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="AI2" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="AJ2" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="AK2" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="AL2" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="AM2" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="AN2" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="AO2" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="AP2" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="AQ2" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="AR2" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="AS2" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="AT2" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="AU2" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="AV2" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="AW2" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="AX2" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="AY2" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="AZ2" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="BA2" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="BB2" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="BC2" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="BD2" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="BE2" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="BF2" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="BG2" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="BH2" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="BI2" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="BJ2" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="BK2" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="BL2" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="BM2" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="BN2" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="BO2" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="BP2" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="BQ2" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="BR2" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="BS2" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="BT2" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="BU2" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="BV2" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="BW2" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="BX2" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="BY2" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="BZ2" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="CA2" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="CB2" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="CC2" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="CD2" s="12" t="s">
-        <v>178</v>
-      </c>
     </row>
-    <row r="3" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="str">
         <f>HYPERLINK("https://classroom.google.com/c/NzE5NDMyNzExMjE5", UPPER("Abrir Classroom"))</f>
         <v>ABRIR CLASSROOM</v>
@@ -1756,8 +1762,11 @@
       <c r="CD3" s="2">
         <v>100</v>
       </c>
+      <c r="CE3" s="12" t="s">
+        <v>107</v>
+      </c>
     </row>
-    <row r="4" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -2004,8 +2013,11 @@
       <c r="CD4" s="6" t="s">
         <v>1</v>
       </c>
+      <c r="CE4" s="12" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="5" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -2330,8 +2342,11 @@
         <f t="shared" ref="CD5" si="75">AVERAGE(CD6:CD38)</f>
         <v>49.151515151515149</v>
       </c>
+      <c r="CE5" s="12" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="6" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>9</v>
       </c>
@@ -2578,8 +2593,11 @@
       <c r="CD6" s="10">
         <v>0</v>
       </c>
+      <c r="CE6" s="12" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="7" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
@@ -2826,8 +2844,11 @@
       <c r="CD7" s="10">
         <v>0</v>
       </c>
+      <c r="CE7" s="12" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="8" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
@@ -3074,8 +3095,11 @@
       <c r="CD8" s="10">
         <v>100</v>
       </c>
+      <c r="CE8" s="12" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="9" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
@@ -3322,8 +3346,11 @@
       <c r="CD9" s="10">
         <v>0</v>
       </c>
+      <c r="CE9" s="12" t="s">
+        <v>113</v>
+      </c>
     </row>
-    <row r="10" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>21</v>
       </c>
@@ -3570,8 +3597,11 @@
       <c r="CD10" s="10">
         <v>100</v>
       </c>
+      <c r="CE10" s="12" t="s">
+        <v>114</v>
+      </c>
     </row>
-    <row r="11" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>24</v>
       </c>
@@ -3818,8 +3848,11 @@
       <c r="CD11" s="10">
         <v>85</v>
       </c>
+      <c r="CE11" s="12" t="s">
+        <v>115</v>
+      </c>
     </row>
-    <row r="12" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>27</v>
       </c>
@@ -4066,8 +4099,11 @@
       <c r="CD12" s="10">
         <v>0</v>
       </c>
+      <c r="CE12" s="12" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="13" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>30</v>
       </c>
@@ -4314,8 +4350,11 @@
       <c r="CD13" s="10">
         <v>0</v>
       </c>
+      <c r="CE13" s="12" t="s">
+        <v>117</v>
+      </c>
     </row>
-    <row r="14" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>32</v>
       </c>
@@ -4562,8 +4601,11 @@
       <c r="CD14" s="10">
         <v>40</v>
       </c>
+      <c r="CE14" s="12" t="s">
+        <v>118</v>
+      </c>
     </row>
-    <row r="15" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>35</v>
       </c>
@@ -4810,8 +4852,11 @@
       <c r="CD15" s="10">
         <v>100</v>
       </c>
+      <c r="CE15" s="12" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="16" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
         <v>38</v>
       </c>
@@ -5058,8 +5103,11 @@
       <c r="CD16" s="10">
         <v>60</v>
       </c>
+      <c r="CE16" s="12" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="17" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>41</v>
       </c>
@@ -5306,8 +5354,11 @@
       <c r="CD17" s="10">
         <v>100</v>
       </c>
+      <c r="CE17" s="12" t="s">
+        <v>121</v>
+      </c>
     </row>
-    <row r="18" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>44</v>
       </c>
@@ -5554,8 +5605,11 @@
       <c r="CD18" s="10">
         <v>0</v>
       </c>
+      <c r="CE18" s="12" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="19" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>47</v>
       </c>
@@ -5802,8 +5856,11 @@
       <c r="CD19" s="10">
         <v>80</v>
       </c>
+      <c r="CE19" s="12" t="s">
+        <v>123</v>
+      </c>
     </row>
-    <row r="20" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>50</v>
       </c>
@@ -6050,8 +6107,11 @@
       <c r="CD20" s="10">
         <v>0</v>
       </c>
+      <c r="CE20" s="12" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="21" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>53</v>
       </c>
@@ -6298,8 +6358,11 @@
       <c r="CD21" s="10">
         <v>90</v>
       </c>
+      <c r="CE21" s="12" t="s">
+        <v>125</v>
+      </c>
     </row>
-    <row r="22" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>56</v>
       </c>
@@ -6546,8 +6609,11 @@
       <c r="CD22" s="10">
         <v>90</v>
       </c>
+      <c r="CE22" s="12" t="s">
+        <v>126</v>
+      </c>
     </row>
-    <row r="23" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
         <v>59</v>
       </c>
@@ -6794,8 +6860,11 @@
       <c r="CD23" s="10">
         <v>90</v>
       </c>
+      <c r="CE23" s="12" t="s">
+        <v>127</v>
+      </c>
     </row>
-    <row r="24" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>62</v>
       </c>
@@ -7042,8 +7111,11 @@
       <c r="CD24" s="10">
         <v>70</v>
       </c>
+      <c r="CE24" s="12" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="25" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>65</v>
       </c>
@@ -7290,8 +7362,11 @@
       <c r="CD25" s="10">
         <v>0</v>
       </c>
+      <c r="CE25" s="12" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="26" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
         <v>68</v>
       </c>
@@ -7538,8 +7613,11 @@
       <c r="CD26" s="10">
         <v>100</v>
       </c>
+      <c r="CE26" s="12" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="27" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>70</v>
       </c>
@@ -7786,8 +7864,11 @@
       <c r="CD27" s="10">
         <v>70</v>
       </c>
+      <c r="CE27" s="12" t="s">
+        <v>131</v>
+      </c>
     </row>
-    <row r="28" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
         <v>73</v>
       </c>
@@ -8034,8 +8115,11 @@
       <c r="CD28" s="10">
         <v>0</v>
       </c>
+      <c r="CE28" s="12" t="s">
+        <v>131</v>
+      </c>
     </row>
-    <row r="29" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>76</v>
       </c>
@@ -8282,8 +8366,11 @@
       <c r="CD29" s="10">
         <v>0</v>
       </c>
+      <c r="CE29" s="12" t="s">
+        <v>132</v>
+      </c>
     </row>
-    <row r="30" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
         <v>79</v>
       </c>
@@ -8530,8 +8617,11 @@
       <c r="CD30" s="10">
         <v>0</v>
       </c>
+      <c r="CE30" s="12" t="s">
+        <v>132</v>
+      </c>
     </row>
-    <row r="31" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
         <v>82</v>
       </c>
@@ -8778,8 +8868,11 @@
       <c r="CD31" s="10">
         <v>90</v>
       </c>
+      <c r="CE31" s="12" t="s">
+        <v>133</v>
+      </c>
     </row>
-    <row r="32" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
         <v>85</v>
       </c>
@@ -9026,8 +9119,11 @@
       <c r="CD32" s="10">
         <v>0</v>
       </c>
+      <c r="CE32" s="12" t="s">
+        <v>133</v>
+      </c>
     </row>
-    <row r="33" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="10" t="s">
         <v>87</v>
       </c>
@@ -9274,8 +9370,11 @@
       <c r="CD33" s="10">
         <v>0</v>
       </c>
+      <c r="CE33" s="12" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="34" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
         <v>90</v>
       </c>
@@ -9522,8 +9621,11 @@
       <c r="CD34" s="10">
         <v>100</v>
       </c>
+      <c r="CE34" s="12" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="35" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
         <v>93</v>
       </c>
@@ -9770,8 +9872,11 @@
       <c r="CD35" s="10">
         <v>97</v>
       </c>
+      <c r="CE35" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
-    <row r="36" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="10" t="s">
         <v>96</v>
       </c>
@@ -10018,8 +10123,11 @@
       <c r="CD36" s="10">
         <v>0</v>
       </c>
+      <c r="CE36" s="12" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="37" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="10" t="s">
         <v>99</v>
       </c>
@@ -10266,8 +10374,11 @@
       <c r="CD37" s="10">
         <v>60</v>
       </c>
+      <c r="CE37" s="12" t="s">
+        <v>137</v>
+      </c>
     </row>
-    <row r="38" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="10" t="s">
         <v>102</v>
       </c>
@@ -10514,49 +10625,212 @@
       <c r="CD38" s="10">
         <v>100</v>
       </c>
+      <c r="CE38" s="12" t="s">
+        <v>138</v>
+      </c>
     </row>
-    <row r="39" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="43" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="44" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="45" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="47" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="48" spans="1:82" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="49" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="50" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="51" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="52" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="53" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="54" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="55" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="56" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="57" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="58" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="59" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="60" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="61" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="62" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="63" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="64" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="65" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="66" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="67" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="68" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="69" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="70" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="71" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="72" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="73" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="74" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="75" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="76" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="77" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="78" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="79" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="80" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE39" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE40" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE41" s="12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE42" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE43" s="12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE44" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE45" s="12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="46" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE46" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="47" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE47" s="12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="48" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE48" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="49" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE49" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="50" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE50" s="12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE51" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE52" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE53" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="54" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE54" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="55" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE55" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE56" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="57" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE57" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="58" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE58" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="59" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE59" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="60" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE60" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="61" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE61" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="62" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE62" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="63" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE63" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="64" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE64" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="65" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE65" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="66" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE66" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="67" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE67" s="12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="68" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE68" s="12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="69" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE69" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="70" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE70" s="12" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="71" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE71" s="12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="72" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE72" s="12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="73" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE73" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="74" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE74" s="12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="75" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE75" s="12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="76" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE76" s="12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="77" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE77" s="12" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="78" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CE78" s="12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="79" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="80" spans="83:83" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="81" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="82" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="83" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
[ADD] it fucking works
</commit_message>
<xml_diff>
--- a/app/utilities/calificaciones1.xlsx
+++ b/app/utilities/calificaciones1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Desktop\Lyra\app\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABCE8DC-C66E-46FF-9473-C76B5B6301E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CCEBEC-E6C5-4EF7-A823-042AD3660445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1028,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CE1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BM1" zoomScale="63" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="BX8" sqref="BX8"/>
+    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>